<commit_message>
Added BulkLoad, new spreadsheet for sample data
</commit_message>
<xml_diff>
--- a/spreadsheets/Portfolio.xlsx
+++ b/spreadsheets/Portfolio.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" firstSheet="2" activeTab="9"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Portfolio" sheetId="2" r:id="rId1"/>
@@ -18,12 +18,12 @@
     <sheet name="TimeSeries" sheetId="8" r:id="rId9"/>
     <sheet name="TimeSeriesMapping" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" calcCompleted="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="100">
   <si>
     <t>Portfolio</t>
   </si>
@@ -31,9 +31,6 @@
     <t>Trade</t>
   </si>
   <si>
-    <t xml:space="preserve">  Portfolio</t>
-  </si>
-  <si>
     <t>Quantity</t>
   </si>
   <si>
@@ -320,6 +317,12 @@
   </si>
   <si>
     <t>SPrating</t>
+  </si>
+  <si>
+    <t>Equity Portfolio 1</t>
+  </si>
+  <si>
+    <t>InstrumentId</t>
   </si>
 </sst>
 </file>
@@ -671,13 +674,13 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -685,21 +688,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" t="s">
         <v>72</v>
-      </c>
-      <c r="B2" t="s">
-        <v>73</v>
       </c>
       <c r="G2" t="str">
         <f>CONCATENATE("CREATE TABLE INFORISK_",A1," (  ",A2,A3,D1,",",B2,B3," )")</f>
@@ -708,15 +711,15 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" t="s">
         <v>67</v>
-      </c>
-      <c r="B3" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -724,7 +727,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -737,7 +740,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -749,56 +752,56 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" t="s">
         <v>63</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>64</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>65</v>
-      </c>
-      <c r="G2" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -806,10 +809,10 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -855,10 +858,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -878,63 +881,63 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" t="s">
         <v>74</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
         <v>75</v>
       </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" t="s">
-        <v>6</v>
-      </c>
       <c r="H2" t="s">
-        <v>7</v>
+        <v>99</v>
       </c>
       <c r="K2" t="str">
         <f>CONCATENATE("CREATE TABLE INFORISK_",A1," (  ",A2,A3,D1,",",B2,B3,",",C2,C3,",",D2,D3,",",E2,E3,",",F2,F3,",",G2,G3,",",H2,H3," )")</f>
-        <v>CREATE TABLE INFORISK_Trade (  PortfolioId int   PRIMARY KEY,TradeId int,Quantity int,Notional float,NotionalUSD float,MarketValue float,MarketValueUSD float,Instrument int )</v>
+        <v>CREATE TABLE INFORISK_Trade (  PortfolioId int   PRIMARY KEY,TradeId int,Quantity int,Notional float,NotionalUSD float,MarketValue float,MarketValueUSD float,InstrumentId int )</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1033,6 +1036,48 @@
       </c>
       <c r="H10">
         <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="str">
+        <f>CONCATENATE("INSERT INTO INFOCUBE.INFORISK_",$A$1," (", $A$2, ", ", $B$2,  ",",  $C$2, ",",  $H$2, ") VALUES (",A4, ",", B4, ",", C4, ",", H4, ");")</f>
+        <v>INSERT INTO INFOCUBE.INFORISK_Trade (PortfolioId, TradeId,Quantity,InstrumentId) VALUES (1,1,100,1);</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="str">
+        <f t="shared" ref="A14:A20" si="0">CONCATENATE("INSERT INTO INFOCUBE.INFORISK_",$A$1," (", $A$2, ", ", $B$2,  ",",  $C$2, ",",  $H$2, ") VALUES (",A5, ",", B5, ",", C5, ",", H5, ");")</f>
+        <v>INSERT INTO INFOCUBE.INFORISK_Trade (PortfolioId, TradeId,Quantity,InstrumentId) VALUES (1,2,100,2);</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO INFOCUBE.INFORISK_Trade (PortfolioId, TradeId,Quantity,InstrumentId) VALUES (1,3,100,3);</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO INFOCUBE.INFORISK_Trade (PortfolioId, TradeId,Quantity,InstrumentId) VALUES (1,4,100,4);</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO INFOCUBE.INFORISK_Trade (PortfolioId, TradeId,Quantity,InstrumentId) VALUES (1,5,100,5);</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO INFOCUBE.INFORISK_Trade (PortfolioId, TradeId,Quantity,InstrumentId) VALUES (1,6,100,6);</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO INFOCUBE.INFORISK_Trade (PortfolioId, TradeId,Quantity,InstrumentId) VALUES (1,7,100,7);</v>
       </c>
     </row>
   </sheetData>
@@ -1059,44 +1104,44 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" t="s">
         <v>78</v>
       </c>
-      <c r="B2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>79</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>80</v>
-      </c>
-      <c r="E2" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3" t="s">
         <v>92</v>
       </c>
-      <c r="D3" t="s">
-        <v>93</v>
-      </c>
       <c r="E3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1107,7 +1152,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1124,7 +1169,7 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -1141,7 +1186,7 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D6">
         <v>3</v>
@@ -1158,7 +1203,7 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D7">
         <v>4</v>
@@ -1175,7 +1220,7 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D8">
         <v>5</v>
@@ -1192,7 +1237,7 @@
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D9">
         <v>6</v>
@@ -1209,7 +1254,7 @@
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D10">
         <v>7</v>
@@ -1231,10 +1276,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1245,74 +1290,74 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" t="s">
         <v>82</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>83</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>84</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>85</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>86</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>87</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>88</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>89</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>90</v>
-      </c>
-      <c r="J2" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F3" t="s">
         <v>92</v>
       </c>
-      <c r="C3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D3" t="s">
-        <v>92</v>
-      </c>
-      <c r="E3" t="s">
-        <v>92</v>
-      </c>
-      <c r="F3" t="s">
-        <v>93</v>
-      </c>
       <c r="G3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1320,7 +1365,7 @@
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1328,7 +1373,7 @@
         <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1336,7 +1381,7 @@
         <v>3</v>
       </c>
       <c r="G6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1344,7 +1389,7 @@
         <v>4</v>
       </c>
       <c r="G7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1352,7 +1397,7 @@
         <v>5</v>
       </c>
       <c r="G8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1360,7 +1405,7 @@
         <v>6</v>
       </c>
       <c r="G9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1368,13 +1413,55 @@
         <v>7</v>
       </c>
       <c r="G10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f>CONCATENATE("CREATE TABLE INFORISK_",A1," (  ",A2,A3,,D1,",",B2,B3,",",C2,C3,",",D2,D3,",",E2,E3,",",F2,F3,",",G2,G3,",",H2,H3,",",I2,I3,",",J2,J3," )")</f>
         <v>CREATE TABLE INFORISK_Instrument (  InstrumentId  int  PRIMARY KEY,CUSIP  varchar,SEDOL  varchar,RIC  varchar,ISIN  varchar,Issuer  int,Symbol  varchar,curve  varchar,tenor  varchar,currency  varchar )</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="str">
+        <f>CONCATENATE("INSERT INTO INFOCUBE.INFORISK_",$A$1," (", $A$2, ", ", $G$2, ") VALUES (", A4, ",'", G4, "');")</f>
+        <v>INSERT INTO INFOCUBE.INFORISK_Instrument (InstrumentId , Symbol ) VALUES (1,'AAPL');</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="str">
+        <f t="shared" ref="A23:A28" si="0">CONCATENATE("INSERT INTO INFOCUBE.INFORISK_",$A$1," (", $A$2, ", ", $G$2, ") VALUES (", A5, ",'", G5, "');")</f>
+        <v>INSERT INTO INFOCUBE.INFORISK_Instrument (InstrumentId , Symbol ) VALUES (2,'GOOG');</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO INFOCUBE.INFORISK_Instrument (InstrumentId , Symbol ) VALUES (3,'CSCO');</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO INFOCUBE.INFORISK_Instrument (InstrumentId , Symbol ) VALUES (4,'MSFT');</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO INFOCUBE.INFORISK_Instrument (InstrumentId , Symbol ) VALUES (5,'TSLA');</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO INFOCUBE.INFORISK_Instrument (InstrumentId , Symbol ) VALUES (6,'GE');</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO INFOCUBE.INFORISK_Instrument (InstrumentId , Symbol ) VALUES (7,'AMZN');</v>
       </c>
     </row>
   </sheetData>
@@ -1400,44 +1487,44 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3" t="s">
         <v>92</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>92</v>
-      </c>
-      <c r="D3" t="s">
-        <v>93</v>
-      </c>
-      <c r="E3" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1445,10 +1532,10 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1462,10 +1549,10 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -1479,10 +1566,10 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D6">
         <v>3</v>
@@ -1496,10 +1583,10 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D7">
         <v>4</v>
@@ -1513,10 +1600,10 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -1530,10 +1617,10 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -1547,10 +1634,10 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -1589,44 +1676,44 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>17</v>
-      </c>
-      <c r="E2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1634,7 +1721,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1642,7 +1729,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1650,7 +1737,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1658,7 +1745,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1666,7 +1753,7 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
@@ -1692,44 +1779,44 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
         <v>20</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>21</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>22</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>23</v>
-      </c>
-      <c r="E2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1737,7 +1824,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1745,7 +1832,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1753,7 +1840,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1795,63 +1882,63 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D1" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" t="s">
         <v>28</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>29</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>30</v>
-      </c>
-      <c r="F2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3">
         <v>100</v>
       </c>
       <c r="P3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C4">
         <v>100</v>
       </c>
       <c r="P4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C5">
         <v>100</v>
@@ -1859,10 +1946,10 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6">
         <v>100</v>
@@ -1870,10 +1957,10 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7">
         <v>100</v>
@@ -1881,10 +1968,10 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8">
         <v>100</v>
@@ -1892,10 +1979,10 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C9">
         <v>100</v>
@@ -1927,32 +2014,32 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
         <v>35</v>
-      </c>
-      <c r="C2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" t="s">
         <v>93</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>94</v>
-      </c>
-      <c r="C3" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1964,7 +2051,7 @@
       </c>
       <c r="C4">
         <f ca="1">RANDBETWEEN(600,700)</f>
-        <v>673</v>
+        <v>616</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1976,7 +2063,7 @@
       </c>
       <c r="C5">
         <f t="shared" ref="C5:C23" ca="1" si="0">RANDBETWEEN(600,700)</f>
-        <v>663</v>
+        <v>668</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1988,7 +2075,7 @@
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>648</v>
+        <v>656</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -2000,7 +2087,7 @@
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="I7" t="str">
         <f>CONCATENATE("CREATE TABLE INFORISK_",A1," (  ",A2,A3,,D1,",",B2,B3,",",C2,C3," )")</f>
@@ -2016,7 +2103,7 @@
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>631</v>
+        <v>655</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -2028,7 +2115,7 @@
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>652</v>
+        <v>648</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -2040,7 +2127,7 @@
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>679</v>
+        <v>616</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -2052,7 +2139,7 @@
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="0"/>
-        <v>606</v>
+        <v>630</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -2064,7 +2151,7 @@
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="0"/>
-        <v>626</v>
+        <v>650</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -2076,7 +2163,7 @@
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="0"/>
-        <v>631</v>
+        <v>606</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -2088,7 +2175,7 @@
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="0"/>
-        <v>673</v>
+        <v>633</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -2100,7 +2187,7 @@
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="0"/>
-        <v>682</v>
+        <v>607</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -2112,7 +2199,7 @@
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="0"/>
-        <v>665</v>
+        <v>643</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2124,7 +2211,7 @@
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="0"/>
-        <v>616</v>
+        <v>645</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2136,7 +2223,7 @@
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="0"/>
-        <v>695</v>
+        <v>662</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2148,7 +2235,7 @@
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="0"/>
-        <v>661</v>
+        <v>690</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2160,7 +2247,7 @@
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="0"/>
-        <v>626</v>
+        <v>601</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2172,7 +2259,7 @@
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="0"/>
-        <v>698</v>
+        <v>691</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2184,7 +2271,7 @@
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="0"/>
-        <v>668</v>
+        <v>635</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -2196,7 +2283,7 @@
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="0"/>
-        <v>615</v>
+        <v>683</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -2208,7 +2295,7 @@
       </c>
       <c r="C24">
         <f ca="1">RANDBETWEEN(1,50)</f>
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -2220,7 +2307,7 @@
       </c>
       <c r="C25">
         <f t="shared" ref="C25:C31" ca="1" si="1">RANDBETWEEN(1,50)</f>
-        <v>37</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -2232,7 +2319,7 @@
       </c>
       <c r="C26">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -2244,7 +2331,7 @@
       </c>
       <c r="C27">
         <f t="shared" ca="1" si="1"/>
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -2256,7 +2343,7 @@
       </c>
       <c r="C28">
         <f t="shared" ca="1" si="1"/>
-        <v>14</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -2268,7 +2355,7 @@
       </c>
       <c r="C29">
         <f t="shared" ca="1" si="1"/>
-        <v>33</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -2292,7 +2379,7 @@
       </c>
       <c r="C31">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added logic for historic var for instrument and trade
</commit_message>
<xml_diff>
--- a/spreadsheets/Portfolio.xlsx
+++ b/spreadsheets/Portfolio.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Portfolio" sheetId="2" r:id="rId1"/>
@@ -18,12 +18,12 @@
     <sheet name="TimeSeries" sheetId="8" r:id="rId9"/>
     <sheet name="TimeSeriesMapping" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="145621" calcCompleted="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="101">
   <si>
     <t>Portfolio</t>
   </si>
@@ -323,6 +323,9 @@
   </si>
   <si>
     <t>InstrumentId</t>
+  </si>
+  <si>
+    <t>GS</t>
   </si>
 </sst>
 </file>
@@ -671,10 +674,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -728,6 +731,12 @@
       </c>
       <c r="B5" t="s">
         <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="str">
+        <f>CONCATENATE("INSERT INTO INFOCUBE.INFORISK_",$A$1," (", $A$2, ", ", $B$2, ") VALUES (",A5, ", '",B5, "');")</f>
+        <v>INSERT INTO INFOCUBE.INFORISK_Portfolio (PortfolioId , PortfolioName ) VALUES (1, 'Equity Portfolio 1');</v>
       </c>
     </row>
   </sheetData>
@@ -858,10 +867,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -962,7 +971,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="H5">
         <v>2</v>
@@ -976,7 +985,7 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="H6">
         <v>3</v>
@@ -990,7 +999,7 @@
         <v>4</v>
       </c>
       <c r="C7">
-        <v>100</v>
+        <v>250</v>
       </c>
       <c r="H7">
         <v>4</v>
@@ -1004,7 +1013,7 @@
         <v>5</v>
       </c>
       <c r="C8">
-        <v>100</v>
+        <v>225</v>
       </c>
       <c r="H8">
         <v>5</v>
@@ -1018,7 +1027,7 @@
         <v>6</v>
       </c>
       <c r="C9">
-        <v>100</v>
+        <v>175</v>
       </c>
       <c r="H9">
         <v>6</v>
@@ -1032,10 +1041,24 @@
         <v>7</v>
       </c>
       <c r="C10">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="H10">
         <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>75</v>
+      </c>
+      <c r="H11">
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1047,37 +1070,43 @@
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f t="shared" ref="A14:A20" si="0">CONCATENATE("INSERT INTO INFOCUBE.INFORISK_",$A$1," (", $A$2, ", ", $B$2,  ",",  $C$2, ",",  $H$2, ") VALUES (",A5, ",", B5, ",", C5, ",", H5, ");")</f>
-        <v>INSERT INTO INFOCUBE.INFORISK_Trade (PortfolioId, TradeId,Quantity,InstrumentId) VALUES (1,2,100,2);</v>
+        <v>INSERT INTO INFOCUBE.INFORISK_Trade (PortfolioId, TradeId,Quantity,InstrumentId) VALUES (1,2,150,2);</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO INFOCUBE.INFORISK_Trade (PortfolioId, TradeId,Quantity,InstrumentId) VALUES (1,3,100,3);</v>
+        <v>INSERT INTO INFOCUBE.INFORISK_Trade (PortfolioId, TradeId,Quantity,InstrumentId) VALUES (1,3,200,3);</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO INFOCUBE.INFORISK_Trade (PortfolioId, TradeId,Quantity,InstrumentId) VALUES (1,4,100,4);</v>
+        <v>INSERT INTO INFOCUBE.INFORISK_Trade (PortfolioId, TradeId,Quantity,InstrumentId) VALUES (1,4,250,4);</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO INFOCUBE.INFORISK_Trade (PortfolioId, TradeId,Quantity,InstrumentId) VALUES (1,5,100,5);</v>
+        <v>INSERT INTO INFOCUBE.INFORISK_Trade (PortfolioId, TradeId,Quantity,InstrumentId) VALUES (1,5,225,5);</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO INFOCUBE.INFORISK_Trade (PortfolioId, TradeId,Quantity,InstrumentId) VALUES (1,6,100,6);</v>
+        <v>INSERT INTO INFOCUBE.INFORISK_Trade (PortfolioId, TradeId,Quantity,InstrumentId) VALUES (1,6,175,6);</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO INFOCUBE.INFORISK_Trade (PortfolioId, TradeId,Quantity,InstrumentId) VALUES (1,7,100,7);</v>
+        <v>INSERT INTO INFOCUBE.INFORISK_Trade (PortfolioId, TradeId,Quantity,InstrumentId) VALUES (1,7,125,7);</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO INFOCUBE.INFORISK_Trade (PortfolioId, TradeId,Quantity,InstrumentId) VALUES (1,8,75,8);</v>
       </c>
     </row>
   </sheetData>
@@ -1276,10 +1305,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1416,6 +1445,14 @@
         <v>42</v>
       </c>
     </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="G11" t="s">
+        <v>100</v>
+      </c>
+    </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f>CONCATENATE("CREATE TABLE INFORISK_",A1," (  ",A2,A3,,D1,",",B2,B3,",",C2,C3,",",D2,D3,",",E2,E3,",",F2,F3,",",G2,G3,",",H2,H3,",",I2,I3,",",J2,J3," )")</f>
@@ -1462,6 +1499,12 @@
       <c r="A28" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO INFOCUBE.INFORISK_Instrument (InstrumentId , Symbol ) VALUES (7,'AMZN');</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="str">
+        <f>CONCATENATE("INSERT INTO INFOCUBE.INFORISK_",$A$1," (", $A$2, ", ", $G$2, ") VALUES (", A11, ",'", G11, "');")</f>
+        <v>INSERT INTO INFOCUBE.INFORISK_Instrument (InstrumentId , Symbol ) VALUES (8,'GS');</v>
       </c>
     </row>
   </sheetData>
@@ -1473,7 +1516,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
@@ -2051,7 +2094,7 @@
       </c>
       <c r="C4">
         <f ca="1">RANDBETWEEN(600,700)</f>
-        <v>616</v>
+        <v>679</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -2063,7 +2106,7 @@
       </c>
       <c r="C5">
         <f t="shared" ref="C5:C23" ca="1" si="0">RANDBETWEEN(600,700)</f>
-        <v>668</v>
+        <v>627</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -2075,7 +2118,7 @@
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>656</v>
+        <v>626</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -2087,7 +2130,7 @@
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>695</v>
+        <v>686</v>
       </c>
       <c r="I7" t="str">
         <f>CONCATENATE("CREATE TABLE INFORISK_",A1," (  ",A2,A3,,D1,",",B2,B3,",",C2,C3," )")</f>
@@ -2103,7 +2146,7 @@
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>655</v>
+        <v>605</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -2115,7 +2158,7 @@
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>648</v>
+        <v>611</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -2127,7 +2170,7 @@
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>616</v>
+        <v>629</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -2139,7 +2182,7 @@
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="0"/>
-        <v>630</v>
+        <v>671</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -2151,7 +2194,7 @@
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="0"/>
-        <v>650</v>
+        <v>621</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -2163,7 +2206,7 @@
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="0"/>
-        <v>606</v>
+        <v>670</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -2175,7 +2218,7 @@
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="0"/>
-        <v>633</v>
+        <v>671</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -2187,7 +2230,7 @@
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="0"/>
-        <v>607</v>
+        <v>613</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -2199,7 +2242,7 @@
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="0"/>
-        <v>643</v>
+        <v>681</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2211,7 +2254,7 @@
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="0"/>
-        <v>645</v>
+        <v>692</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2223,7 +2266,7 @@
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="0"/>
-        <v>662</v>
+        <v>687</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2235,7 +2278,7 @@
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="0"/>
-        <v>690</v>
+        <v>693</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2247,7 +2290,7 @@
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="0"/>
-        <v>601</v>
+        <v>691</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2259,7 +2302,7 @@
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="0"/>
-        <v>691</v>
+        <v>683</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2271,7 +2314,7 @@
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="0"/>
-        <v>635</v>
+        <v>629</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -2283,7 +2326,7 @@
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="0"/>
-        <v>683</v>
+        <v>690</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -2295,7 +2338,7 @@
       </c>
       <c r="C24">
         <f ca="1">RANDBETWEEN(1,50)</f>
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -2307,7 +2350,7 @@
       </c>
       <c r="C25">
         <f t="shared" ref="C25:C31" ca="1" si="1">RANDBETWEEN(1,50)</f>
-        <v>7</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -2319,7 +2362,7 @@
       </c>
       <c r="C26">
         <f t="shared" ca="1" si="1"/>
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -2331,7 +2374,7 @@
       </c>
       <c r="C27">
         <f t="shared" ca="1" si="1"/>
-        <v>33</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -2343,7 +2386,7 @@
       </c>
       <c r="C28">
         <f t="shared" ca="1" si="1"/>
-        <v>27</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -2355,7 +2398,7 @@
       </c>
       <c r="C29">
         <f t="shared" ca="1" si="1"/>
-        <v>17</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -2367,7 +2410,7 @@
       </c>
       <c r="C30">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -2379,7 +2422,7 @@
       </c>
       <c r="C31">
         <f t="shared" ca="1" si="1"/>
-        <v>20</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>